<commit_message>
Added environment setups for R code
</commit_message>
<xml_diff>
--- a/isolate-table.xlsx
+++ b/isolate-table.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kasperstorck/Documents/01 IRTLab/00 Colabs-repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE53975B-1B86-0A47-AED8-1E5ECA9E95BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D138A8-1727-7C41-82B0-EAF8FF6EF86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="760" windowWidth="28040" windowHeight="17240" xr2:uid="{C2F3B680-5C20-424F-86DD-519CF26F4CE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -609,7 +609,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added scripts to handle gene qPCR and calculating relative abundance
</commit_message>
<xml_diff>
--- a/isolate-table.xlsx
+++ b/isolate-table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kasperstorck/Documents/01 IRTLab/00 Colabs-repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D138A8-1727-7C41-82B0-EAF8FF6EF86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4650FF8-2B8F-6D47-B7D2-2E6FDC26C1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="760" windowWidth="28040" windowHeight="17240" xr2:uid="{C2F3B680-5C20-424F-86DD-519CF26F4CE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="62">
   <si>
     <t>KS-01</t>
   </si>
@@ -207,6 +207,21 @@
   </si>
   <si>
     <t>Unknown</t>
+  </si>
+  <si>
+    <t>Helper strain</t>
+  </si>
+  <si>
+    <t>Form colonies on carbon-free agar plate</t>
+  </si>
+  <si>
+    <t>Many</t>
+  </si>
+  <si>
+    <t>Few</t>
+  </si>
+  <si>
+    <t>Very few</t>
   </si>
 </sst>
 </file>
@@ -609,7 +624,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -637,6 +652,12 @@
       <c r="F1" t="s">
         <v>41</v>
       </c>
+      <c r="G1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -657,6 +678,12 @@
       <c r="F2" t="s">
         <v>38</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -676,6 +703,12 @@
       </c>
       <c r="F3" t="s">
         <v>38</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="I3" s="3"/>
       <c r="K3" s="2"/>
@@ -707,6 +740,12 @@
       <c r="F4" t="s">
         <v>43</v>
       </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" t="s">
+        <v>60</v>
+      </c>
       <c r="I4" s="3"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -737,6 +776,12 @@
       <c r="F5" t="s">
         <v>39</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -767,6 +812,12 @@
       <c r="F6" t="s">
         <v>43</v>
       </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" t="s">
+        <v>60</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -797,6 +848,12 @@
       <c r="F7" t="s">
         <v>39</v>
       </c>
+      <c r="G7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="I7" s="3"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -827,6 +884,12 @@
       <c r="F8" t="s">
         <v>38</v>
       </c>
+      <c r="G8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="I8" s="3"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -857,6 +920,12 @@
       <c r="F9" t="s">
         <v>38</v>
       </c>
+      <c r="G9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="I9" s="3"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -887,6 +956,12 @@
       <c r="F10" t="s">
         <v>39</v>
       </c>
+      <c r="G10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="I10" s="3"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -917,6 +992,12 @@
       <c r="F11" t="s">
         <v>43</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="I11" s="3"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -947,6 +1028,12 @@
       <c r="F12" t="s">
         <v>39</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="I12" s="3"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -977,6 +1064,12 @@
       <c r="F13" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="I13" s="3"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -1007,6 +1100,12 @@
       <c r="F14" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="I14" s="3"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -1037,6 +1136,12 @@
       <c r="F15" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="I15" s="3"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -1067,6 +1172,12 @@
       <c r="F16" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="I16" s="3"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -1097,6 +1208,12 @@
       <c r="F17" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="I17" s="3"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -1127,6 +1244,12 @@
       <c r="F18" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="I18" s="3"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -1157,6 +1280,12 @@
       <c r="F19" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="I19" s="3"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -1187,6 +1316,12 @@
       <c r="F20" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="I20" s="3"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -1217,6 +1352,12 @@
       <c r="F21" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="I21" s="3"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -1247,6 +1388,12 @@
       <c r="F22" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="I22" s="3"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
@@ -1277,6 +1424,12 @@
       <c r="F23" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="I23" s="3"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
@@ -1307,6 +1460,12 @@
       <c r="F24" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="I24" s="3"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
@@ -1337,6 +1496,12 @@
       <c r="F25" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="I25" s="3"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -1367,6 +1532,12 @@
       <c r="F26" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="I26" s="3"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -1397,6 +1568,12 @@
       <c r="F27" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="I27" s="3"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
@@ -1427,6 +1604,12 @@
       <c r="F28" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="I28" s="3"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -1457,6 +1640,12 @@
       <c r="F29" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>